<commit_message>
All but one test passes.
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -56,7 +56,7 @@
     <t>D*</t>
   </si>
   <si>
-    <t>&lt;S</t>
+    <t>S&lt;</t>
   </si>
   <si>
     <t>S^</t>
@@ -250,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -279,6 +279,12 @@
     <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
@@ -294,14 +300,11 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="12" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="1" fillId="13" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="12" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="1" fillId="13" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -918,7 +921,7 @@
       <c r="H5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="10" t="s">
         <v>14</v>
       </c>
       <c r="J5" s="7" t="s">
@@ -1182,7 +1185,7 @@
       <c r="D8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="11" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="7" t="s">
@@ -1512,7 +1515,7 @@
       <c r="V11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W11" s="10" t="s">
+      <c r="W11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="X11" s="4" t="s">
@@ -1642,10 +1645,10 @@
       <c r="D13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="4" t="s">
+      <c r="E13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>20</v>
       </c>
       <c r="G13" s="7" t="s">
@@ -1728,22 +1731,22 @@
       <c r="B14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="4" t="s">
+      <c r="C14" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="11" t="s">
         <v>20</v>
       </c>
       <c r="I14" s="7" t="s">
@@ -1817,28 +1820,28 @@
       <c r="A15" s="2">
         <v>13.0</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="4" t="s">
+      <c r="B15" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>20</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I15" s="4" t="s">
+      <c r="F15" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" s="11" t="s">
         <v>20</v>
       </c>
       <c r="J15" s="7" t="s">
@@ -1909,31 +1912,31 @@
       <c r="A16" s="2">
         <v>14.0</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="B16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>20</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" s="9" t="s">
+      <c r="F16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="10" t="s">
         <v>14</v>
       </c>
       <c r="K16" s="7" t="s">
@@ -2001,28 +2004,28 @@
       <c r="A17" s="2">
         <v>15.0</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I17" s="4" t="s">
+      <c r="B17" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="11" t="s">
         <v>20</v>
       </c>
       <c r="J17" s="7" t="s">
@@ -2070,7 +2073,7 @@
       <c r="X17" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y17" s="10" t="s">
+      <c r="Y17" s="12" t="s">
         <v>18</v>
       </c>
       <c r="Z17" s="4" t="s">
@@ -2096,22 +2099,22 @@
       <c r="B18" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="4" t="s">
+      <c r="C18" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="11" t="s">
         <v>20</v>
       </c>
       <c r="I18" s="7" t="s">
@@ -2194,10 +2197,10 @@
       <c r="D19" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="4" t="s">
+      <c r="E19" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="11" t="s">
         <v>20</v>
       </c>
       <c r="G19" s="7" t="s">
@@ -2524,7 +2527,7 @@
       <c r="V22" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W22" s="11" t="s">
+      <c r="W22" s="13" t="s">
         <v>5</v>
       </c>
       <c r="X22" s="4" t="s">
@@ -2533,13 +2536,13 @@
       <c r="Y22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Z22" s="10" t="s">
+      <c r="Z22" s="12" t="s">
         <v>5</v>
       </c>
       <c r="AA22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AB22" s="10" t="s">
+      <c r="AB22" s="12" t="s">
         <v>15</v>
       </c>
       <c r="AC22" s="5" t="s">
@@ -2553,19 +2556,19 @@
       <c r="A23" s="2">
         <v>21.0</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" s="4" t="s">
+      <c r="B23" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="11" t="s">
         <v>26</v>
       </c>
       <c r="G23" s="7" t="s">
@@ -2642,25 +2645,25 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="12">
+      <c r="A24" s="14">
         <v>22.0</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G24" s="4" t="s">
+      <c r="B24" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="11" t="s">
         <v>26</v>
       </c>
       <c r="H24" s="7" t="s">
@@ -2684,19 +2687,19 @@
       <c r="N24" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="O24" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="P24" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q24" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="R24" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="S24" s="4" t="s">
+      <c r="O24" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P24" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q24" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="R24" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S24" s="11" t="s">
         <v>27</v>
       </c>
       <c r="T24" s="9" t="s">
@@ -2734,28 +2737,28 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="12">
+      <c r="A25" s="14">
         <v>23.0</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H25" s="4" t="s">
+      <c r="B25" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H25" s="11" t="s">
         <v>26</v>
       </c>
       <c r="I25" s="7" t="s">
@@ -2776,22 +2779,22 @@
       <c r="N25" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="O25" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="P25" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q25" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="R25" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="S25" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="T25" s="4" t="s">
+      <c r="O25" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P25" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q25" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="R25" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S25" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="T25" s="11" t="s">
         <v>27</v>
       </c>
       <c r="U25" s="7" t="s">
@@ -2806,19 +2809,19 @@
       <c r="X25" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="Y25" s="4" t="s">
+      <c r="Y25" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="Z25" s="10" t="s">
+      <c r="Z25" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AA25" s="4" t="s">
+      <c r="AA25" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AB25" s="10" t="s">
+      <c r="AB25" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AC25" s="4" t="s">
+      <c r="AC25" s="11" t="s">
         <v>28</v>
       </c>
       <c r="AD25" s="5" t="s">
@@ -2826,31 +2829,31 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="12">
+      <c r="A26" s="14">
         <v>24.0</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I26" s="4" t="s">
+      <c r="B26" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I26" s="11" t="s">
         <v>26</v>
       </c>
       <c r="J26" s="7" t="s">
@@ -2865,25 +2868,25 @@
       <c r="M26" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="N26" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="O26" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="P26" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q26" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="R26" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="S26" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="T26" s="4" t="s">
+      <c r="N26" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O26" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P26" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q26" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="R26" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S26" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="T26" s="11" t="s">
         <v>27</v>
       </c>
       <c r="U26" s="7" t="s">
@@ -2895,25 +2898,25 @@
       <c r="W26" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="X26" s="4" t="s">
+      <c r="X26" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="Y26" s="4" t="s">
+      <c r="Y26" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="Z26" s="4" t="s">
+      <c r="Z26" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AA26" s="4" t="s">
+      <c r="AA26" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AB26" s="4" t="s">
+      <c r="AB26" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AC26" s="4" t="s">
+      <c r="AC26" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AD26" s="4" t="s">
+      <c r="AD26" s="11" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2921,34 +2924,34 @@
       <c r="A27" s="2">
         <v>25.0</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="4" t="s">
+      <c r="B27" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="11" t="s">
         <v>26</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K27" s="9" t="s">
+      <c r="F27" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K27" s="10" t="s">
         <v>14</v>
       </c>
       <c r="L27" s="7" t="s">
@@ -2957,25 +2960,25 @@
       <c r="M27" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="N27" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="O27" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="P27" s="4" t="s">
+      <c r="N27" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O27" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P27" s="11" t="s">
         <v>27</v>
       </c>
       <c r="Q27" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="R27" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="S27" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="T27" s="4" t="s">
+      <c r="R27" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S27" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="T27" s="11" t="s">
         <v>27</v>
       </c>
       <c r="U27" s="7" t="s">
@@ -2987,25 +2990,25 @@
       <c r="W27" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="X27" s="10" t="s">
+      <c r="X27" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Y27" s="4" t="s">
+      <c r="Y27" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="Z27" s="4" t="s">
+      <c r="Z27" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AA27" s="4" t="s">
+      <c r="AA27" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AB27" s="4" t="s">
+      <c r="AB27" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AC27" s="4" t="s">
+      <c r="AC27" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AD27" s="4" t="s">
+      <c r="AD27" s="11" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3013,31 +3016,31 @@
       <c r="A28" s="2">
         <v>26.0</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="4" t="s">
+      <c r="B28" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>26</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J28" s="4" t="s">
+      <c r="E28" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I28" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J28" s="11" t="s">
         <v>26</v>
       </c>
       <c r="K28" s="5" t="s">
@@ -3049,25 +3052,25 @@
       <c r="M28" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="N28" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="O28" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="P28" s="4" t="s">
+      <c r="N28" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O28" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P28" s="11" t="s">
         <v>27</v>
       </c>
       <c r="Q28" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="R28" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="S28" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="T28" s="4" t="s">
+      <c r="R28" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S28" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="T28" s="11" t="s">
         <v>27</v>
       </c>
       <c r="U28" s="7" t="s">
@@ -3079,25 +3082,25 @@
       <c r="W28" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="X28" s="4" t="s">
+      <c r="X28" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="Y28" s="4" t="s">
+      <c r="Y28" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="Z28" s="4" t="s">
+      <c r="Z28" s="11" t="s">
         <v>28</v>
       </c>
       <c r="AA28" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="AB28" s="4" t="s">
+      <c r="AB28" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AC28" s="4" t="s">
+      <c r="AC28" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AD28" s="4" t="s">
+      <c r="AD28" s="11" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3105,31 +3108,31 @@
       <c r="A29" s="2">
         <v>27.0</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J29" s="4" t="s">
+      <c r="B29" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I29" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J29" s="11" t="s">
         <v>26</v>
       </c>
       <c r="K29" s="5" t="s">
@@ -3138,31 +3141,31 @@
       <c r="L29" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="M29" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N29" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="O29" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="P29" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q29" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="R29" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="S29" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="T29" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="U29" s="4" t="s">
+      <c r="M29" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N29" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O29" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P29" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q29" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="R29" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S29" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="T29" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U29" s="11" t="s">
         <v>34</v>
       </c>
       <c r="V29" s="5" t="s">
@@ -3174,22 +3177,22 @@
       <c r="X29" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="Y29" s="4" t="s">
+      <c r="Y29" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="Z29" s="4" t="s">
+      <c r="Z29" s="11" t="s">
         <v>28</v>
       </c>
       <c r="AA29" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AB29" s="4" t="s">
+      <c r="AB29" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AC29" s="4" t="s">
+      <c r="AC29" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AD29" s="4" t="s">
+      <c r="AD29" s="11" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3197,31 +3200,31 @@
       <c r="A30" s="2">
         <v>28.0</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J30" s="4" t="s">
+      <c r="C30" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J30" s="11" t="s">
         <v>26</v>
       </c>
       <c r="K30" s="5" t="s">
@@ -3230,31 +3233,31 @@
       <c r="L30" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="M30" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N30" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="O30" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="P30" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q30" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="R30" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="S30" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="T30" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="U30" s="13" t="s">
+      <c r="M30" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N30" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O30" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P30" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q30" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="R30" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S30" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="T30" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U30" s="15" t="s">
         <v>34</v>
       </c>
       <c r="V30" s="5" t="s">
@@ -3263,25 +3266,25 @@
       <c r="W30" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="X30" s="4" t="s">
+      <c r="X30" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="Y30" s="4" t="s">
+      <c r="Y30" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="Z30" s="4" t="s">
+      <c r="Z30" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AA30" s="4" t="s">
+      <c r="AA30" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AB30" s="4" t="s">
+      <c r="AB30" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AC30" s="4" t="s">
+      <c r="AC30" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AD30" s="4" t="s">
+      <c r="AD30" s="11" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3306,60 +3309,60 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
-      <c r="B1" s="14">
+      <c r="B1" s="16">
         <v>0.0</v>
       </c>
-      <c r="C1" s="14">
+      <c r="C1" s="16">
         <v>1.0</v>
       </c>
-      <c r="D1" s="14">
+      <c r="D1" s="16">
         <v>2.0</v>
       </c>
-      <c r="E1" s="14">
+      <c r="E1" s="16">
         <v>3.0</v>
       </c>
-      <c r="F1" s="15"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" ht="30.0" customHeight="1">
-      <c r="A2" s="14">
+      <c r="A2" s="16">
         <v>0.0</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" ht="30.0" customHeight="1">
-      <c r="A3" s="14">
+      <c r="A3" s="16">
         <v>1.0</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="15"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" ht="30.0" customHeight="1">
-      <c r="A4" s="15">
+      <c r="A4" s="16">
         <v>2.0</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="16"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="17"/>
     </row>
     <row r="5" ht="30.0" customHeight="1">
-      <c r="A5" s="15">
+      <c r="A5" s="16">
         <v>3.0</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
     </row>
     <row r="6" ht="15.0" customHeight="1">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
added missing files to repo
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -536,7 +536,7 @@
   <dimension ref="A1:AD30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH14" sqref="AH14"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -633,7 +633,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="19">
         <v>0</v>
       </c>
@@ -725,7 +725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="19">
         <v>1</v>
       </c>
@@ -817,7 +817,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="19">
         <v>2</v>
       </c>
@@ -909,7 +909,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="19">
         <v>3</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="19">
         <v>4</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="19">
         <v>5</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="19">
         <v>6</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="19">
         <v>7</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="19">
         <v>8</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="19">
         <v>9</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="19">
         <v>10</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="19">
         <v>11</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="19">
         <v>12</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="19">
         <v>13</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="19">
         <v>14</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="19">
         <v>15</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="19">
         <v>16</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="19">
         <v>17</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="19">
         <v>18</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="19">
         <v>19</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="19">
         <v>20</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="19">
         <v>21</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="19">
         <v>22</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="19">
         <v>23</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="19">
         <v>24</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="19">
         <v>25</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="19">
         <v>26</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="19">
         <v>27</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="19">
         <v>28</v>
       </c>

</xml_diff>